<commit_message>
complete first 11 trials
</commit_message>
<xml_diff>
--- a/cleaned_data/meta_data.xlsx
+++ b/cleaned_data/meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEA31C0-DEAF-4FF1-89A9-BFC1431C8219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F09E0C-4FFF-4FFD-ACC9-3E57E4F28184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>trial_id</t>
   </si>
@@ -79,9 +79,6 @@
 Fisher's exact test</t>
   </si>
   <si>
-    <t>NCT03000348(CARE-CF-1)</t>
-  </si>
-  <si>
     <t>Oral cysteamine as an adjunct treatment in cystic fibrosis pulmonary exacerbations: An exploratory randomized clinical trial</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
   </si>
   <si>
     <t>https://peerj.com/articles/10709/</t>
-  </si>
-  <si>
-    <t>countinuous</t>
   </si>
   <si>
     <t>No, primary outcomes not significantly different</t>
@@ -153,13 +147,173 @@
   </si>
   <si>
     <t># of arm</t>
+  </si>
+  <si>
+    <t>Village-wide prophylaxis arm:
+Significant reduction in attack rate compared to the control arm
+Household prophylaxis arm:
+No significant difference from the control arm</t>
+  </si>
+  <si>
+    <t>Cluster-level t-tests (log-transformed ARs)
+Poisson regression with overdispersion adjustment for adjusted AR ratios
+Mixed-effects logistic regression for individual-level effectiveness
+Linear regression with generalized estimating equations (GEE) for resistance sub-study</t>
+  </si>
+  <si>
+    <t>UMIN000004490</t>
+  </si>
+  <si>
+    <t>The Effect of Sitagliptin on Carotid Artery Atherosclerosis in Type 2 Diabetes: The PROLOGUE Randomized Controlled Trial</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pmed.1002051</t>
+  </si>
+  <si>
+    <t>No. The difference in IMT change was not statistically significant</t>
+  </si>
+  <si>
+    <t>ANCOVA
+Mixed-effects model for repeated measures (as sensitivity analysis)</t>
+  </si>
+  <si>
+    <t>NCT03000348</t>
+  </si>
+  <si>
+    <t>Exploratory data on the clinical efficacy of monoclonal antibodies against SARS-CoV-2 Omicron variant of concern</t>
+  </si>
+  <si>
+    <t>https://elifesciences.org/articles/79639</t>
+  </si>
+  <si>
+    <t>NCT05205759</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Composite binary outcome</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">No, the trial did not succeed in demonstrating a significant difference in the primary outcome (COVID-19 progression through day 14) between treatment arms
+Additionally, the trial was </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>underpowered</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> due to early discontinuation (only ~25% of target sample enrolled), which limited its ability to detect non-inferiority or superiority.</t>
+    </r>
+  </si>
+  <si>
+    <t>Kaplan-Meier estimator and Cox proportional hazard model
+Log-rank tests
+Wilcoxon and Fisher’s exact tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paired t-tests (main comparisons between DDD-60 and DDD-80)
+Wilcoxon signed-rank test (nonparametric sensitivity)
+Two-way repeated measures ANOVA
+</t>
+  </si>
+  <si>
+    <t>MSNA burst incidence significantly decreased at 80 bpm (mean: 51 vs 64 bursts/100 RR, p &lt; 0.05)
+NT-proBNP: no significant difference (p = 0.3 by paired t-test; p = 0.44 by ANOVA)</t>
+  </si>
+  <si>
+    <t>Optimal Cardiac Resynchronization Therapy Pacing Rate in Non-Ischemic Heart Failure Patients: A Randomized Crossover Pilot Trial</t>
+  </si>
+  <si>
+    <t>NCT02258061</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0138124</t>
+  </si>
+  <si>
+    <t>NCT04379336</t>
+  </si>
+  <si>
+    <t>No,HR = 2.0 (95% CI 0.69–5.9), p = 0.20</t>
+  </si>
+  <si>
+    <t>Safety and efficacy of BCG re-vaccination in relation to
+COVID-19 morbidity in healthcare workers: A doubleblind, randomised, controlled, phase 3 trial</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.
+eclinm.2022.101414</t>
+  </si>
+  <si>
+    <t>Cox proportional hazards model
+time-to-event analyses
+post hoc Markovian analysis</t>
+  </si>
+  <si>
+    <t>Binary time-to-event</t>
+  </si>
+  <si>
+    <t>NCT02050360</t>
+  </si>
+  <si>
+    <t>On-Demand Sildenafil as a Treatment for Raynaud Phenomenon
+A Series of n-of-1 Trials</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.7326/M18-0517</t>
+  </si>
+  <si>
+    <t>2/3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No (at population level):
+High individual-level probability of sildenafil &gt; placebo (≥90%)
+But aggregated effect size was not clinically relevant
+ Yes (for select individuals):
+Some participants showed clinically meaningful improvement
+</t>
+  </si>
+  <si>
+    <t>Bayesian mixed-effects models
+Outcomes estimated using adjusted relative variation (aRV)
+Model covariates included sex, age, temperature, humidity, RP type, and CCB use
+Aggregated and individual probabilities of superiority calculated</t>
+  </si>
+  <si>
+    <t>https://bmjopen.bmj.com/content/11/12/e050271</t>
+  </si>
+  <si>
+    <t>NCT02252588</t>
+  </si>
+  <si>
+    <t>Chlorhexidine oral rinses for symptomatic COPD: a randomised, blind, placebo-controlled preliminary study</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No, the trial did not meet its primary outcome. There was no statistically significant difference in oral or sputum microbiota biomass between the chlorhexidine and placebo groups (oral microbiota p=0.665; sputum microbiota p=0.096 without imputation, p=0.078 with imputation)</t>
+  </si>
+  <si>
+    <t>Primary analysis: Two-sample t-test on log10-transformed biomass data, with multiple imputation for missing sputum weights
+Secondary analyses: Linear regression models for biodiversity indices, BCSS, SGRQ and inflammatory markers, with each model adjusted for the baseline value of the measure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +356,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -238,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -262,8 +423,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,14 +715,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -557,7 +730,7 @@
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
@@ -574,7 +747,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>4</v>
@@ -583,7 +756,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>6</v>
@@ -656,18 +829,18 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row r="3" spans="1:26" ht="240">
+    <row r="3" spans="1:26" ht="150">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -679,13 +852,13 @@
         <v>400</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -708,14 +881,14 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="3">
         <v>6</v>
@@ -730,10 +903,10 @@
         <v>11</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -757,13 +930,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -775,13 +948,13 @@
         <v>75</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -800,25 +973,37 @@
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
     </row>
-    <row r="6" spans="1:26" ht="75">
+    <row r="6" spans="1:26" ht="180">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>297</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -836,19 +1021,37 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" ht="60">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3">
+        <v>463</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -866,19 +1069,37 @@
       <c r="Y7" s="4"/>
       <c r="Z7" s="4"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" ht="165">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="B8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="3">
+        <v>311</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -896,19 +1117,37 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="120">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="B9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>12</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -926,19 +1165,37 @@
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" ht="75">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="B10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -956,19 +1213,37 @@
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" ht="165">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="3">
+        <v>38</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -986,19 +1261,37 @@
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" ht="135">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>44</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>

</xml_diff>

<commit_message>
add uptill trial 14
</commit_message>
<xml_diff>
--- a/cleaned_data/meta_data.xlsx
+++ b/cleaned_data/meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F09E0C-4FFF-4FFD-ACC9-3E57E4F28184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067506DB-77E5-439A-A46F-505E7ADC4B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,31 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
-  <si>
-    <t>trial_id</t>
-  </si>
-  <si>
-    <t>trial name</t>
-  </si>
-  <si>
-    <t>paper name</t>
-  </si>
-  <si>
-    <t>paper link</t>
-  </si>
-  <si>
-    <t>phase</t>
-  </si>
-  <si>
-    <t>sample size</t>
-  </si>
-  <si>
-    <t>trial success</t>
-  </si>
-  <si>
-    <t>statistical model</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="90">
   <si>
     <t>NCT02491333</t>
   </si>
@@ -66,9 +42,6 @@
   </si>
   <si>
     <t>https://doi.org/10.1093/humrep/deab272</t>
-  </si>
-  <si>
-    <t>continuous</t>
   </si>
   <si>
     <t>No, the primary outcome is not signicantly better</t>
@@ -107,9 +80,6 @@
     <t xml:space="preserve">independent t-test
 quantile regression
 </t>
-  </si>
-  <si>
-    <t>primary outcome type</t>
   </si>
   <si>
     <t>NCT04523831</t>
@@ -144,9 +114,6 @@
   </si>
   <si>
     <t>https://doi.org/10.1371/journal.pmed.1002593</t>
-  </si>
-  <si>
-    <t># of arm</t>
   </si>
   <si>
     <t>Village-wide prophylaxis arm:
@@ -305,8 +272,108 @@
     <t xml:space="preserve"> No, the trial did not meet its primary outcome. There was no statistically significant difference in oral or sputum microbiota biomass between the chlorhexidine and placebo groups (oral microbiota p=0.665; sputum microbiota p=0.096 without imputation, p=0.078 with imputation)</t>
   </si>
   <si>
+    <t>PACTR201105000289276</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0114602</t>
+  </si>
+  <si>
     <t>Primary analysis: Two-sample t-test on log10-transformed biomass data, with multiple imputation for missing sputum weights
 Secondary analyses: Linear regression models for biodiversity indices, BCSS, SGRQ and inflammatory markers, with each model adjusted for the baseline value of the measure</t>
+  </si>
+  <si>
+    <t>Wilcoxon rank-sum test (between arms)
+Wilcoxon signed-rank test (within-person change)
+Linear regression for slope of CD4 and viral load change</t>
+  </si>
+  <si>
+    <t>NCT02954068</t>
+  </si>
+  <si>
+    <t>Does route matter? Impact of route of oxytocin administration on postpartum bleeding: A double-blind, randomized controlled trial</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0222981</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Binary (proportion with blood loss ≥ 500 ml)
+Continuous (mean blood loss in ml)</t>
+  </si>
+  <si>
+    <t>Categorical variables: Pearson χ² or Fisher’s exact tests
+Continuous variables: Independent t-tests or Mann-Whitney U tests (depending on normality)</t>
+  </si>
+  <si>
+    <t>Safety and Immunogenicity of H1/IC31H,
+an Adjuvanted TB Subunit Vaccine, in HIV-Infected Adults with CD4+ Lymphocyte
+Counts Greater than 350 cells/mm3: A
+Phase II, Multi-Centre, Double-Blind,
+Randomized, Placebo-Controlled Trial</t>
+  </si>
+  <si>
+    <t>ChiCTR2000031834</t>
+  </si>
+  <si>
+    <t>A telerehabilitation programme in post-discharge
+COVID-19 patients (TERECO): a randomised
+controlled trial</t>
+  </si>
+  <si>
+    <t>https://thorax.bmj.com/content/77/7/697</t>
+  </si>
+  <si>
+    <t>Control Group</t>
+  </si>
+  <si>
+    <t>Trial_ID</t>
+  </si>
+  <si>
+    <t>trial Registration Number</t>
+  </si>
+  <si>
+    <t>Paper Name</t>
+  </si>
+  <si>
+    <t>Paper Link</t>
+  </si>
+  <si>
+    <t># of Arm</t>
+  </si>
+  <si>
+    <t>Study Phase</t>
+  </si>
+  <si>
+    <t>Sample Size</t>
+  </si>
+  <si>
+    <t>Primary Outcome Type</t>
+  </si>
+  <si>
+    <t>Trial Success</t>
+  </si>
+  <si>
+    <t>Statistical Model</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>No Active Rehabilitation</t>
+  </si>
+  <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>Priamry Outcome</t>
+  </si>
+  <si>
+    <t>6-minute walking distance (6MWD) in meters at 6 weeks (post-treatment) and at follow-up (~28 weeks)</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -399,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -429,14 +496,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,59 +786,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" customWidth="1"/>
+    <col min="10" max="10" width="40.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="44.42578125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="38.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" customHeight="1">
+    <row r="1" spans="1:28" ht="18" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
+        <v>78</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>23</v>
+        <v>79</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
@@ -780,40 +859,42 @@
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
-    </row>
-    <row r="2" spans="1:26" ht="60">
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+    </row>
+    <row r="2" spans="1:28" ht="60">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E2" s="3">
         <v>3</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
         <v>3</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>342</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -828,40 +909,42 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
-    </row>
-    <row r="3" spans="1:26" ht="150">
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+    </row>
+    <row r="3" spans="1:28" ht="150">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
         <v>3</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>400</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>19</v>
+      </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
@@ -876,40 +959,42 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
-    </row>
-    <row r="4" spans="1:26" ht="45">
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+    </row>
+    <row r="4" spans="1:28" ht="45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E4" s="3">
         <v>6</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
         <v>2</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>89</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -924,40 +1009,42 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
-    </row>
-    <row r="5" spans="1:26" ht="60">
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+    </row>
+    <row r="5" spans="1:28" ht="60">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>75</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -972,40 +1059,42 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
-    </row>
-    <row r="6" spans="1:26" ht="180">
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+    </row>
+    <row r="6" spans="1:28" ht="180">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
         <v>4</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>297</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1020,40 +1109,42 @@
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
-    </row>
-    <row r="7" spans="1:26" ht="60">
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+    </row>
+    <row r="7" spans="1:28" ht="60">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
         <v>4</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>463</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="I7" s="3"/>
       <c r="J7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -1068,40 +1159,42 @@
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
       <c r="Z7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="165">
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+    </row>
+    <row r="8" spans="1:28" ht="135">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E8" s="3">
         <v>3</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="F8" s="3"/>
+      <c r="G8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="3">
         <v>311</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="I8" s="3"/>
       <c r="J8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1116,40 +1209,42 @@
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" ht="120">
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+    </row>
+    <row r="9" spans="1:28" ht="120">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>51</v>
+        <v>41</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E9" s="3">
         <v>2</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>12</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1164,40 +1259,42 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="75">
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+    </row>
+    <row r="10" spans="1:28" ht="75">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>56</v>
+        <v>43</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E10" s="3">
         <v>2</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F10" s="3"/>
+      <c r="G10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="3">
         <v>1000</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="I10" s="3"/>
       <c r="J10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1212,40 +1309,42 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
-    </row>
-    <row r="11" spans="1:26" ht="165">
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+    </row>
+    <row r="11" spans="1:28" ht="165">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>62</v>
+        <v>49</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="E11" s="3">
         <v>3</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="F11" s="3"/>
+      <c r="G11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="3">
         <v>38</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1260,40 +1359,42 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="135">
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+    </row>
+    <row r="12" spans="1:28" ht="150">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>66</v>
+        <v>56</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="E12" s="3">
         <v>2</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3">
         <v>2</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>44</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="I12" s="3"/>
       <c r="J12" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1308,22 +1409,42 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
-    </row>
-    <row r="13" spans="1:26">
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+    </row>
+    <row r="13" spans="1:28" ht="105">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2</v>
+      </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>48</v>
+      </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="J13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>62</v>
+      </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1338,22 +1459,42 @@
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
-    </row>
-    <row r="14" spans="1:26">
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+    </row>
+    <row r="14" spans="1:28" ht="90">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2</v>
+      </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="G14" s="3">
+        <v>4</v>
+      </c>
+      <c r="H14" s="3">
+        <v>543</v>
+      </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="J14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1368,23 +1509,47 @@
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
       <c r="Z14" s="4"/>
-    </row>
-    <row r="15" spans="1:26">
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+    </row>
+    <row r="15" spans="1:28" ht="60">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="B15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="3">
+        <v>119</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="12"/>
+      <c r="M15" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -1398,8 +1563,10 @@
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
-    </row>
-    <row r="16" spans="1:26">
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4"/>
+    </row>
+    <row r="16" spans="1:28">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1412,8 +1579,8 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -1428,13 +1595,15 @@
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
       <c r="Z16" s="4"/>
-    </row>
-    <row r="17" spans="1:26">
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+    </row>
+    <row r="17" spans="1:28">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -1442,8 +1611,8 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -1458,13 +1627,15 @@
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
-    </row>
-    <row r="18" spans="1:26">
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+    </row>
+    <row r="18" spans="1:28">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1472,8 +1643,8 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -1488,13 +1659,15 @@
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
       <c r="Z18" s="4"/>
-    </row>
-    <row r="19" spans="1:26">
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+    </row>
+    <row r="19" spans="1:28">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1502,8 +1675,8 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -1518,13 +1691,15 @@
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
-    </row>
-    <row r="20" spans="1:26">
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+    </row>
+    <row r="20" spans="1:28">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1532,8 +1707,8 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -1548,13 +1723,15 @@
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
       <c r="Z20" s="4"/>
-    </row>
-    <row r="21" spans="1:26">
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
+    </row>
+    <row r="21" spans="1:28">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1562,8 +1739,8 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -1578,13 +1755,15 @@
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
-    </row>
-    <row r="22" spans="1:26">
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+    </row>
+    <row r="22" spans="1:28">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1592,8 +1771,8 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -1608,13 +1787,15 @@
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
       <c r="Z22" s="4"/>
-    </row>
-    <row r="23" spans="1:26">
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+    </row>
+    <row r="23" spans="1:28">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1622,8 +1803,8 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -1638,6 +1819,8 @@
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
       <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
compete uptill trial 18
</commit_message>
<xml_diff>
--- a/cleaned_data/meta_data.xlsx
+++ b/cleaned_data/meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067506DB-77E5-439A-A46F-505E7ADC4B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5FBEEB-1D3E-4A99-B82E-AD6C3B284C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
   <si>
     <t>NCT02491333</t>
   </si>
@@ -299,10 +299,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Binary (proportion with blood loss ≥ 500 ml)
-Continuous (mean blood loss in ml)</t>
-  </si>
-  <si>
     <t>Categorical variables: Pearson χ² or Fisher’s exact tests
 Continuous variables: Independent t-tests or Mann-Whitney U tests (depending on normality)</t>
   </si>
@@ -331,9 +327,6 @@
     <t>Trial_ID</t>
   </si>
   <si>
-    <t>trial Registration Number</t>
-  </si>
-  <si>
     <t>Paper Name</t>
   </si>
   <si>
@@ -352,9 +345,6 @@
     <t>Primary Outcome Type</t>
   </si>
   <si>
-    <t>Trial Success</t>
-  </si>
-  <si>
     <t>Statistical Model</t>
   </si>
   <si>
@@ -374,18 +364,130 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>For primary outcome and most secondary continuous outcomes: Constrained longitudinal data analysis (linear mixed effects model with equality constraint on baseline means), adjusted for center (fixed effect) with random intercept for participants
+For mMRC-dyspnoea: Generalized linear model of the Poisson family with a log link, adjusted for center and using natural logarithm of the number of observed occasions as offset, with cluster robust standard errors</t>
+  </si>
+  <si>
+    <t>Conventional Only</t>
+  </si>
+  <si>
+    <t>Proportion with Blood Loss ≥ 500: Binary
+Mean Blood Loss: Continuous</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ctim.2025.103139</t>
+  </si>
+  <si>
+    <t>The effect of Snoezelen intervention on problem behaviors in children with cerebral palsy: A randomized controlled trial</t>
+  </si>
+  <si>
+    <t>KCT0002794</t>
+  </si>
+  <si>
+    <t>Trial Number</t>
+  </si>
+  <si>
+    <t>Change in Child Behavior Checklist (CBCL 1.5–5) scores (pre- vs. post-intervention)</t>
+  </si>
+  <si>
+    <t>Trial Success(Primary Outcome Significant)</t>
+  </si>
+  <si>
+    <t>Within-group: Wilcoxon signed-rank test
+Between-group: Mann-Whitney U test
+Correlation: Spearman’s rank correlation (ρ)
+Association: Linear regression (R² for GMFCS vs. change in emotional reactivity)</t>
+  </si>
+  <si>
+    <t>Waitlist</t>
+  </si>
+  <si>
+    <t>NCT01573130</t>
+  </si>
+  <si>
+    <t>Internet-delivered therapist-guided
+physical activity for mild to moderate
+depression: a randomized controlled trial</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.7717/peerj.178</t>
+  </si>
+  <si>
+    <t>Reduction in depressive symptoms as measured by the Beck Depression Inventory-II (BDI-II)</t>
+  </si>
+  <si>
+    <t>Two-way mixed ANOVA (group × time)</t>
+  </si>
+  <si>
+    <t>The Effectiveness and Safety of Intensive Lipid-Lowering with
+Different Rosuvastatin-Based Regimens in Patients at High
+Cardiovascular Disease Risk: A Nonblind, Randomized, Controlled
+Trial</t>
+  </si>
+  <si>
+    <t>ChiCTR2200058389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://doi.org/10.31083/j.rcm2408222</t>
+  </si>
+  <si>
+    <t>Statin</t>
+  </si>
+  <si>
+    <t>Change in lipid levels (total cholesterol and LDL-C) from baseline at 24 weeks</t>
+  </si>
+  <si>
+    <t>Within-group changes: Wilcoxon signed-rank test with rank-biserial correlation
+Between-group comparisons: Kruskal–Wallis one-way ANOVA with Dunn’s post-hoc test
+Target-achievement analysis: Multivariate logistic regression (adjusting for covariates)</t>
+  </si>
+  <si>
+    <t>Disengagement: Time-to-event
+Time in care: Continuous proportion</t>
+  </si>
+  <si>
+    <t>NCT02474992</t>
+  </si>
+  <si>
+    <t>The Kanyakla study: Randomized controlled trial of a microclinic social network intervention for promoting engagement and retention in HIV care in rural western Kenya</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0255945</t>
+  </si>
+  <si>
+    <t>Usual Care</t>
+  </si>
+  <si>
+    <t>Time to disengagement: first ≥90-day absence from any HIV care visit in 12 months
+Time in care: proportion of time adherent to appointments over 12 months</t>
+  </si>
+  <si>
+    <t>Disengagement: Cox proportional hazards
+Time in Care: linear regression with bootstrapping
+Continuous outcomes (social support, stigma): linear regression with 10,000-replication bootstrap, adjusting for baseline.
+Disclosure counts: Poisson regression, adjusting for baseline, with robust SE for clustering</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -466,50 +568,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,62 +891,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" style="13" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.5703125" customWidth="1"/>
-    <col min="10" max="10" width="40.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="44.42578125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="38.7109375" style="14" customWidth="1"/>
+    <col min="10" max="10" width="38.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.42578125" style="13" customWidth="1"/>
+    <col min="12" max="12" width="38.7109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="18" customHeight="1">
       <c r="A1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="K1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
@@ -869,7 +972,7 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -887,12 +990,12 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="M2" s="4"/>
@@ -919,7 +1022,7 @@
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -939,10 +1042,10 @@
       <c r="J3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="12" t="s">
         <v>19</v>
       </c>
       <c r="M3" s="4"/>
@@ -969,7 +1072,7 @@
       <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -987,12 +1090,12 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>8</v>
       </c>
       <c r="M4" s="4"/>
@@ -1012,14 +1115,14 @@
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
     </row>
-    <row r="5" spans="1:28" ht="60">
+    <row r="5" spans="1:28" ht="45">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1037,12 +1140,12 @@
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K5" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>13</v>
       </c>
       <c r="M5" s="4"/>
@@ -1069,7 +1172,7 @@
       <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1087,12 +1190,12 @@
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K6" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="4"/>
@@ -1119,7 +1222,7 @@
       <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1137,12 +1240,12 @@
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K7" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="11" t="s">
         <v>29</v>
       </c>
       <c r="M7" s="4"/>
@@ -1169,7 +1272,7 @@
       <c r="B8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1189,10 +1292,10 @@
       <c r="J8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="12" t="s">
         <v>37</v>
       </c>
       <c r="M8" s="4"/>
@@ -1219,10 +1322,10 @@
       <c r="B9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="3">
@@ -1237,12 +1340,12 @@
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K9" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="12" t="s">
         <v>38</v>
       </c>
       <c r="M9" s="4"/>
@@ -1269,7 +1372,7 @@
       <c r="B10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1289,10 +1392,10 @@
       <c r="J10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="12" t="s">
         <v>47</v>
       </c>
       <c r="M10" s="4"/>
@@ -1319,7 +1422,7 @@
       <c r="B11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1329,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="10" t="s">
         <v>52</v>
       </c>
       <c r="H11" s="3">
@@ -1337,12 +1440,12 @@
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="11" t="s">
         <v>54</v>
       </c>
       <c r="M11" s="4"/>
@@ -1369,7 +1472,7 @@
       <c r="B12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -1387,12 +1490,12 @@
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K12" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="K12" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="11" t="s">
         <v>61</v>
       </c>
       <c r="M12" s="4"/>
@@ -1419,8 +1522,8 @@
       <c r="B13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>69</v>
+      <c r="C13" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>60</v>
@@ -1437,12 +1540,12 @@
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="11" t="s">
         <v>62</v>
       </c>
       <c r="M13" s="4"/>
@@ -1469,7 +1572,7 @@
       <c r="B14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="11" t="s">
         <v>64</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1487,13 +1590,13 @@
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -1512,43 +1615,45 @@
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
     </row>
-    <row r="15" spans="1:28" ht="60">
+    <row r="15" spans="1:28" ht="210">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="D15" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>72</v>
       </c>
       <c r="E15" s="3">
         <v>2</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H15" s="3">
         <v>119</v>
       </c>
-      <c r="I15" s="12" t="s">
-        <v>88</v>
+      <c r="I15" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="J15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -1566,22 +1671,46 @@
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" ht="150">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="3">
+        <v>28</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -1598,22 +1727,46 @@
       <c r="AA16" s="4"/>
       <c r="AB16" s="4"/>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" ht="60">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="4"/>
+      <c r="B17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="3">
+        <v>48</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -1630,22 +1783,46 @@
       <c r="AA17" s="4"/>
       <c r="AB17" s="4"/>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" ht="150">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="4"/>
+      <c r="B18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="3">
+        <v>4</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="3">
+        <v>294</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -1662,22 +1839,46 @@
       <c r="AA18" s="4"/>
       <c r="AB18" s="4"/>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" ht="210">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="4"/>
+      <c r="B19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="3">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="3">
+        <v>295</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -1699,7 +1900,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="12"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1707,8 +1908,8 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -1731,7 +1932,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="12"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1739,8 +1940,8 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -1763,7 +1964,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="12"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1771,8 +1972,8 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -1795,7 +1996,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="12"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1803,8 +2004,8 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>

</xml_diff>

<commit_message>
complete all basic data cleaning
</commit_message>
<xml_diff>
--- a/cleaned_data/meta_data.xlsx
+++ b/cleaned_data/meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54763904-9DCB-4ECC-93ED-E057C9E5DF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF672D81-4AB1-4D48-9231-D2D9F4C9DFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-101" yWindow="-101" windowWidth="29002" windowHeight="15682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="208">
   <si>
     <t>NCT02491333</t>
   </si>
@@ -118,33 +118,6 @@
     </r>
   </si>
   <si>
-    <t>NCT02050360</t>
-  </si>
-  <si>
-    <t>On-Demand Sildenafil as a Treatment for Raynaud Phenomenon
-A Series of n-of-1 Trials</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.7326/M18-0517</t>
-  </si>
-  <si>
-    <t>2/3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No (at population level):
-High individual-level probability of sildenafil &gt; placebo (≥90%)
-But aggregated effect size was not clinically relevant
- Yes (for select individuals):
-Some participants showed clinically meaningful improvement
-</t>
-  </si>
-  <si>
-    <t>Bayesian mixed-effects models
-Outcomes estimated using adjusted relative variation (aRV)
-Model covariates included sex, age, temperature, humidity, RP type, and CCB use
-Aggregated and individual probabilities of superiority calculated</t>
-  </si>
-  <si>
     <t>https://bmjopen.bmj.com/content/11/12/e050271</t>
   </si>
   <si>
@@ -225,9 +198,6 @@
   </si>
   <si>
     <t>6-minute walking distance (6MWD) in meters at 6 weeks (post-treatment) and at follow-up (~28 weeks)</t>
-  </si>
-  <si>
-    <t>ok</t>
   </si>
   <si>
     <t>For primary outcome and most secondary continuous outcomes: Constrained longitudinal data analysis (linear mixed effects model with equality constraint on baseline means), adjusted for center (fixed effect) with random intercept for participants
@@ -647,9 +617,6 @@
     <t>Sham acupuncture + placebo</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>Primary: Kaplan–Meier survival curves + log-rank test; Cox proportional hazards regression for hazard ratios
 Secondary: Logistic regression for categorical recovery time and disease progression</t>
   </si>
@@ -808,6 +775,32 @@
   <si>
     <t>Binary outcomes: logistic regression with cluster-robust standard errors
 Continuous outcomes: ordinary least squares regression with cluster-robust standard errors</t>
+  </si>
+  <si>
+    <t>NCT02926144</t>
+  </si>
+  <si>
+    <t>Influence of videolaryngoscopy using
+McGrath Mac on the need for a helper
+to perform intubation during general
+anaesthesia: a multicentre randomised
+video-no-video trial</t>
+  </si>
+  <si>
+    <t>10.1136/bmjopen-2021-049275</t>
+  </si>
+  <si>
+    <t>No Video</t>
+  </si>
+  <si>
+    <t>Proportion of orotracheal intubations requiring assistance at the operator’s request</t>
+  </si>
+  <si>
+    <t>Primary outcome (binary): comparison of proportions by χ² test (with Bonferroni correction for multiple comparisons when assessing IDS components).
+Secondary categorical outcomes: χ² or Fisher’s exact tests (as appropriate).
+Continuous outcomes (e.g., POGO, time): Wilcoxon rank-sum test (after verifying normality with Shapiro–Wilk).
+Intubation Difficulty Scale (ordinal): Wilcoxon or χ² for class comparisons.
+Hemodynamic changes: pre- vs post-intubation medians compared by Wilcoxon; between-group differences tested similarly.</t>
   </si>
 </sst>
 </file>
@@ -973,7 +966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1062,9 +1055,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1345,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.65"/>
@@ -1368,43 +1358,43 @@
   <sheetData>
     <row r="1" spans="1:29" ht="18" customHeight="1">
       <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="L1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
@@ -1440,32 +1430,30 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G2" s="3">
         <v>3</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I2" s="3">
         <v>342</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>165</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -1499,19 +1487,19 @@
         <v>2</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I3" s="3">
         <v>400</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>9</v>
@@ -1520,11 +1508,9 @@
         <v>10</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="N3" s="34" t="s">
-        <v>52</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="N3" s="34"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -1546,44 +1532,42 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I4" s="3">
         <v>6030</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="N4" s="34" t="s">
-        <v>52</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="N4" s="34"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
@@ -1617,32 +1601,30 @@
         <v>2</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G5" s="3">
         <v>2</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I5" s="3">
         <v>75</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="N5" s="34" t="s">
-        <v>52</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="N5" s="34"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
@@ -1664,44 +1646,42 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E6" s="3">
         <v>2</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I6" s="3">
         <v>5060</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="N6" s="34" t="s">
-        <v>52</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="N6" s="34"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
@@ -1735,32 +1715,30 @@
         <v>2</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G7" s="3">
         <v>4</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I7" s="3">
         <v>463</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="N7" s="34" t="s">
-        <v>52</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="N7" s="34"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
@@ -1794,19 +1772,19 @@
         <v>3</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I8" s="3">
         <v>311</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>18</v>
@@ -1815,11 +1793,9 @@
         <v>19</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="N8" s="34" t="s">
-        <v>52</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="N8" s="34"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -1841,44 +1817,42 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E9" s="3">
         <v>2</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I9" s="3">
         <v>115</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
@@ -1900,44 +1874,42 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E10" s="3">
         <v>2</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I10" s="3">
         <v>577</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -1954,39 +1926,45 @@
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
     </row>
-    <row r="11" spans="1:29" ht="160.9">
+    <row r="11" spans="1:29" ht="263.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>202</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>21</v>
+        <v>203</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>204</v>
       </c>
       <c r="E11" s="3">
-        <v>3</v>
-      </c>
-      <c r="F11" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>205</v>
+      </c>
       <c r="G11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="I11" s="3">
-        <v>38</v>
-      </c>
-      <c r="J11" s="3"/>
+        <v>256</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="K11" s="3" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>25</v>
+        <v>207</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -2010,44 +1988,42 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E12" s="3">
         <v>2</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G12" s="3">
         <v>2</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I12" s="3">
         <v>44</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
@@ -2069,22 +2045,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>205</v>
+        <v>196</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>197</v>
       </c>
       <c r="E13" s="3">
         <v>2</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>10</v>
@@ -2093,20 +2069,18 @@
         <v>30</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="N13" s="37" t="s">
-        <v>52</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="N13" s="36"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
@@ -2128,44 +2102,42 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3">
         <v>2</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G14" s="3">
         <v>4</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I14" s="3">
         <v>480</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
@@ -2187,44 +2159,42 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3">
         <v>2</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I15" s="3">
         <v>119</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L15" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
@@ -2246,44 +2216,42 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E16" s="3">
         <v>2</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I16" s="3">
         <v>28</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L16" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="N16" s="13" t="s">
-        <v>52</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="N16" s="13"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
@@ -2305,44 +2273,42 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E17" s="3">
         <v>2</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I17" s="3">
         <v>48</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L17" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
@@ -2364,44 +2330,42 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3">
         <v>4</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I18" s="3">
         <v>294</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L18" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
@@ -2423,44 +2387,42 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E19" s="3">
         <v>2</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I19" s="3">
         <v>295</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
@@ -2482,44 +2444,42 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E20" s="3">
         <v>2</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I20" s="3">
         <v>32</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
@@ -2541,44 +2501,42 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E21" s="3">
         <v>2</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I21" s="3">
         <v>37</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
@@ -2600,44 +2558,42 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E22" s="3">
         <v>3</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I22" s="3">
         <v>1462</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="N22" s="15" t="s">
-        <v>52</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="N22" s="15"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
@@ -2659,44 +2615,42 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E23" s="3">
         <v>2</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I23" s="3">
         <v>25</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L23" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="N23" s="16" t="s">
-        <v>52</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="N23" s="16"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
@@ -2718,87 +2672,82 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E24" s="2">
         <v>2</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H24" s="27" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I24" s="2">
         <v>92</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="K24" s="22" t="s">
         <v>9</v>
       </c>
       <c r="L24" s="23" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M24" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="N24" s="24" t="s">
-        <v>52</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="N24" s="24"/>
     </row>
     <row r="25" spans="1:29" ht="175.5">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E25" s="2">
         <v>2</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I25" s="2">
         <v>50</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="L25" s="18" t="s">
         <v>10</v>
       </c>
       <c r="M25" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="N25" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:29" ht="175.5">
@@ -2806,43 +2755,40 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E26" s="26">
         <v>2</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G26" s="2">
         <v>3</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I26" s="2">
         <v>55</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="K26" s="27" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="L26" s="18" t="s">
         <v>10</v>
       </c>
       <c r="M26" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="N26" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:29" ht="190.15">
@@ -2850,154 +2796,148 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E27" s="2">
         <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I27" s="2">
         <v>242</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="K27" s="28" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L27" s="29" t="s">
         <v>10</v>
       </c>
       <c r="M27" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="N27" s="30" t="s">
-        <v>52</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="N27" s="30"/>
     </row>
     <row r="28" spans="1:29" ht="102.4">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E28" s="2">
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H28" s="27" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I28" s="2">
         <v>101</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M28" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="N28" s="30" t="s">
-        <v>52</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="N28" s="30"/>
     </row>
     <row r="29" spans="1:29" ht="146.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E29" s="2">
         <v>2</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I29" s="2">
         <v>120</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="K29" s="27" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="L29" s="18" t="s">
         <v>10</v>
       </c>
       <c r="M29" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="N29" s="30" t="s">
-        <v>52</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="N29" s="30"/>
     </row>
     <row r="30" spans="1:29" ht="219.4">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E30" s="2">
         <v>2</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>10</v>
@@ -3006,64 +2946,60 @@
         <v>51</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="K30" s="27" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L30" s="32" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="M30" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="N30" s="30" t="s">
-        <v>52</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="N30" s="30"/>
     </row>
     <row r="31" spans="1:29" ht="175.5">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E31" s="2">
         <v>3</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I31" s="2">
         <v>75</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="K31" s="27" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="L31" s="18" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="M31" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="N31" s="33" t="s">
-        <v>52</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="N31" s="33"/>
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="19"/>

</xml_diff>

<commit_message>
update uptill trial 13
</commit_message>
<xml_diff>
--- a/cleaned_data/meta_data.xlsx
+++ b/cleaned_data/meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF676F11-B186-4ED7-978C-0813841C0C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B74C467-D205-4931-98A7-26DD21F3B67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-101" yWindow="-101" windowWidth="29002" windowHeight="15682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="210">
   <si>
     <t>NCT02491333</t>
   </si>
@@ -805,17 +805,27 @@
   <si>
     <t>No(acupuncture was not more effective than metformin or sham acupuncture)</t>
   </si>
+  <si>
+    <t>1, 但有问题</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -976,49 +986,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1030,43 +1040,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -1346,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.65"/>
@@ -1755,7 +1766,9 @@
       <c r="M7" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="N7" s="37"/>
+      <c r="N7" s="37">
+        <v>1</v>
+      </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
@@ -1812,7 +1825,9 @@
       <c r="M8" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="N8" s="37"/>
+      <c r="N8" s="38" t="s">
+        <v>209</v>
+      </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -1869,7 +1884,9 @@
       <c r="M9" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="N9" s="4"/>
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
@@ -1926,7 +1943,9 @@
       <c r="M10" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="N10" s="4"/>
+      <c r="N10" s="4">
+        <v>1</v>
+      </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -1983,7 +2002,9 @@
       <c r="M11" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="N11" s="4"/>
+      <c r="N11" s="4">
+        <v>1</v>
+      </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
@@ -2040,7 +2061,9 @@
       <c r="M12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="4"/>
+      <c r="N12" s="4">
+        <v>1</v>
+      </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
@@ -2154,7 +2177,9 @@
       <c r="M14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="N14" s="4"/>
+      <c r="N14" s="4">
+        <v>1</v>
+      </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>

</xml_diff>

<commit_message>
update up till 27
</commit_message>
<xml_diff>
--- a/cleaned_data/meta_data.xlsx
+++ b/cleaned_data/meta_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183C0090-F495-4FFC-B924-19325D80134A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6127E7-78F7-455F-80B1-6FC1AB2CDE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="210">
   <si>
     <t>NCT02491333</t>
   </si>
@@ -78,44 +79,7 @@
     <t>https://doi.org/10.1371/journal.pmed.1002051</t>
   </si>
   <si>
-    <t>Exploratory data on the clinical efficacy of monoclonal antibodies against SARS-CoV-2 Omicron variant of concern</t>
-  </si>
-  <si>
-    <t>https://elifesciences.org/articles/79639</t>
-  </si>
-  <si>
-    <t>NCT05205759</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Composite binary outcome</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">No, the trial did not succeed in demonstrating a significant difference in the primary outcome (COVID-19 progression through day 14) between treatment arms
-Additionally, the trial was </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>underpowered</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> due to early discontinuation (only ~25% of target sample enrolled), which limited its ability to detect non-inferiority or superiority.</t>
-    </r>
   </si>
   <si>
     <t>https://bmjopen.bmj.com/content/11/12/e050271</t>
@@ -493,9 +457,6 @@
   </si>
   <si>
     <t>Intraoperative bleeding during transsphenoidal pituitary surgery, scored using a 7-level bleeding scale.</t>
-  </si>
-  <si>
-    <t>Ordinal, Categorical</t>
   </si>
   <si>
     <t>Primary outcome: ordinal logistic regression (proportional cumulative odds)
@@ -654,17 +615,6 @@
 Baseline comparisons: unpaired t-tests and Fisher’s exact tests</t>
   </si>
   <si>
-    <t>Casirivimab/Imdevimab</t>
-  </si>
-  <si>
-    <t>Composite COVID-19 progression through day 14 (hospitalization, need for supplemental oxygen, or death)</t>
-  </si>
-  <si>
-    <t>Continuous variables: Wilcoxon–Mann–Whitney test
-Categorical variables: Fisher’s exact test
-Time-to-event analyses (time to symptom resolution): Kaplan–Meier estimator + Log-rank test; Cox proportional hazards model for predictor associations</t>
-  </si>
-  <si>
     <t>Proportion of patients with a negative SARS-CoV-2 RT-PCR on Day 6 post-enrolment</t>
   </si>
   <si>
@@ -816,6 +766,34 @@
   </si>
   <si>
     <t>Symptoms: YS_side_effect_description</t>
+  </si>
+  <si>
+    <t>NCT02927197</t>
+  </si>
+  <si>
+    <t>Comparing Two Methods of Delivering ThinkRx Cognitive Training
+to Children Ages 8–14: a Randomized Controlled Trial of Equivalency</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s41465-018-0094-z</t>
+  </si>
+  <si>
+    <t>ThinkRx</t>
+  </si>
+  <si>
+    <t>Change scores (post – pre) on eight Woodcock–Johnson III cognitive subtests: associative memory, visual processing, auditory processing, logic &amp; reasoning, processing speed, working memory/attention, long-term memory, and general intellectual ability.</t>
+  </si>
+  <si>
+    <t>Primary analysis: MANOVA on difference scores with Bonferroni correction
+Sensitivity: ANCOVA for each post-test controlling baseline; OLS regression with clustered standard errors (for sibling dependence)</t>
+  </si>
+  <si>
+    <t>Equivalence (no significant difference) demonstrated on 7 of 8 measures; however, long-term memory gains were significantly greater in the ThinkRx arm</t>
+  </si>
+  <si>
+    <t>Bleeeding categoriy: Ordinal, Categorical
+Surgical problem bleeding: Binary
+Bleeding Score: Continuous</t>
   </si>
 </sst>
 </file>
@@ -828,6 +806,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -900,13 +885,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -967,104 +945,108 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1343,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="F27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1366,46 +1348,46 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18" customHeight="1">
       <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="J1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="L1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="N1" s="6" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -1438,28 +1420,28 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G2" s="3">
         <v>3</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I2" s="3">
         <v>342</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="N2" s="10"/>
       <c r="O2" s="4">
@@ -1495,19 +1477,19 @@
         <v>2</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3">
         <v>400</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>9</v>
@@ -1516,7 +1498,7 @@
         <v>10</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="N3" s="11"/>
       <c r="O3" s="4">
@@ -1540,40 +1522,40 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I4" s="3">
         <v>6030</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="N4" s="11"/>
       <c r="O4" s="4">
@@ -1609,31 +1591,33 @@
         <v>2</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G5" s="3">
         <v>2</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I5" s="3">
         <v>75</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="N5" s="11"/>
-      <c r="O5" s="4"/>
+      <c r="O5" s="4">
+        <v>1</v>
+      </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
@@ -1652,43 +1636,45 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E6" s="3">
         <v>2</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I6" s="3">
         <v>5060</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="N6" s="11"/>
-      <c r="O6" s="4"/>
+      <c r="O6" s="4">
+        <v>1</v>
+      </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -1719,31 +1705,33 @@
         <v>2</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G7" s="3">
         <v>4</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I7" s="3">
         <v>463</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="N7" s="11"/>
-      <c r="O7" s="4"/>
+      <c r="O7" s="4">
+        <v>1</v>
+      </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -1762,43 +1750,45 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>16</v>
+        <v>202</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>203</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>204</v>
       </c>
       <c r="E8" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I8" s="3">
-        <v>311</v>
+        <v>38</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>19</v>
+        <v>208</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>169</v>
+        <v>207</v>
       </c>
       <c r="N8" s="11"/>
-      <c r="O8" s="4"/>
+      <c r="O8" s="4">
+        <v>1</v>
+      </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -1817,45 +1807,47 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E9" s="3">
         <v>2</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I9" s="3">
         <v>115</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="O9" s="4"/>
+        <v>200</v>
+      </c>
+      <c r="O9" s="4">
+        <v>1</v>
+      </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -1874,45 +1866,47 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E10" s="3">
         <v>2</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I10" s="3">
         <v>577</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="O10" s="4"/>
+        <v>201</v>
+      </c>
+      <c r="O10" s="4">
+        <v>1</v>
+      </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -1931,43 +1925,45 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E11" s="3">
         <v>2</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I11" s="3">
         <v>256</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="N11" s="10"/>
-      <c r="O11" s="4"/>
+      <c r="O11" s="4">
+        <v>1</v>
+      </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
@@ -1986,43 +1982,45 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E12" s="3">
         <v>2</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="G12" s="3">
         <v>2</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I12" s="3">
         <v>44</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="N12" s="10"/>
-      <c r="O12" s="4"/>
+      <c r="O12" s="4">
+        <v>1</v>
+      </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
@@ -2041,22 +2039,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E13" s="3">
         <v>2</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>10</v>
@@ -2065,19 +2063,21 @@
         <v>30</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="N13" s="11"/>
-      <c r="O13" s="4"/>
+      <c r="O13" s="4">
+        <v>1</v>
+      </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
@@ -2096,43 +2096,45 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E14" s="3">
         <v>2</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G14" s="3">
         <v>4</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I14" s="3">
         <v>480</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="N14" s="11"/>
-      <c r="O14" s="4"/>
+      <c r="O14" s="4">
+        <v>1</v>
+      </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -2151,43 +2153,45 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3">
         <v>2</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I15" s="3">
         <v>119</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L15" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N15" s="10"/>
-      <c r="O15" s="4"/>
+      <c r="O15" s="4">
+        <v>1</v>
+      </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
@@ -2206,43 +2210,45 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E16" s="3">
         <v>2</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I16" s="3">
         <v>28</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L16" s="11" t="s">
         <v>10</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="N16" s="11"/>
-      <c r="O16" s="4"/>
+      <c r="O16" s="4">
+        <v>1</v>
+      </c>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
@@ -2261,43 +2267,45 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E17" s="3">
         <v>2</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I17" s="3">
         <v>48</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L17" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N17" s="10"/>
-      <c r="O17" s="4"/>
+      <c r="O17" s="4">
+        <v>1</v>
+      </c>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
@@ -2316,43 +2324,45 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E18" s="3">
         <v>4</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I18" s="3">
         <v>294</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N18" s="10"/>
-      <c r="O18" s="4"/>
+      <c r="O18" s="4">
+        <v>1</v>
+      </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
@@ -2371,43 +2381,45 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E19" s="3">
         <v>2</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I19" s="3">
         <v>295</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N19" s="10"/>
-      <c r="O19" s="4"/>
+      <c r="O19" s="4">
+        <v>1</v>
+      </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
@@ -2426,43 +2438,45 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E20" s="3">
         <v>2</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I20" s="3">
         <v>32</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N20" s="10"/>
-      <c r="O20" s="4"/>
+      <c r="O20" s="4">
+        <v>1</v>
+      </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
@@ -2481,43 +2495,45 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E21" s="3">
         <v>2</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I21" s="3">
         <v>37</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N21" s="10"/>
-      <c r="O21" s="4"/>
+      <c r="O21" s="4">
+        <v>1</v>
+      </c>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
@@ -2536,43 +2552,45 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E22" s="3">
         <v>3</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I22" s="3">
         <v>1462</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="N22" s="29"/>
-      <c r="O22" s="4"/>
+      <c r="O22" s="4">
+        <v>1</v>
+      </c>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
@@ -2591,22 +2609,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="E23" s="3">
         <v>2</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>10</v>
@@ -2615,19 +2633,21 @@
         <v>20</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="N23" s="30"/>
-      <c r="O23" s="4"/>
+      <c r="O23" s="4">
+        <v>1</v>
+      </c>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
@@ -2646,250 +2666,265 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E24" s="2">
         <v>2</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I24" s="2">
         <v>92</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K24" s="18" t="s">
         <v>9</v>
       </c>
       <c r="L24" s="19" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M24" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N24" s="31"/>
+      <c r="O24" s="34">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:27" ht="174">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E25" s="2">
         <v>2</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H25" s="22" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I25" s="2">
         <v>50</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="K25" s="20" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L25" s="14" t="s">
         <v>10</v>
       </c>
       <c r="M25" s="14" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="N25" s="32"/>
+      <c r="O25" s="34">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:27" ht="174">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E26" s="21">
         <v>2</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G26" s="2">
         <v>3</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I26" s="2">
         <v>55</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L26" s="14" t="s">
         <v>10</v>
       </c>
       <c r="M26" s="14" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="N26" s="32"/>
+      <c r="O26" s="34">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:27" ht="174">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E27" s="2">
         <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I27" s="2">
         <v>242</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="K27" s="28" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="L27" s="23" t="s">
         <v>10</v>
       </c>
       <c r="M27" s="23" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N27" s="33"/>
+      <c r="O27" s="34">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:27" ht="101.5">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E28" s="2">
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I28" s="2">
         <v>101</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K28" s="22" t="s">
-        <v>126</v>
+        <v>120</v>
+      </c>
+      <c r="K28" s="35" t="s">
+        <v>209</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M28" s="14" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="N28" s="32"/>
+      <c r="O28" s="34">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:27" ht="145">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E29" s="2">
         <v>2</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I29" s="2">
         <v>120</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="K29" s="22" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L29" s="14" t="s">
         <v>10</v>
       </c>
       <c r="M29" s="14" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="N29" s="32"/>
     </row>
@@ -2898,22 +2933,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E30" s="2">
         <v>2</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>10</v>
@@ -2922,16 +2957,16 @@
         <v>51</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="L30" s="25" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="M30" s="14" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="N30" s="32"/>
     </row>
@@ -2940,40 +2975,40 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E31" s="2">
         <v>3</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I31" s="2">
         <v>75</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="K31" s="27" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L31" s="14" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="M31" s="14" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="N31" s="32"/>
     </row>

</xml_diff>

<commit_message>
update sl and whole rct function
</commit_message>
<xml_diff>
--- a/cleaned_data/meta_data.xlsx
+++ b/cleaned_data/meta_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20479B4-AE95-4F5D-9170-45456FD9AD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BAC352-1259-434E-ACE3-0F8F4C1D2568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -953,7 +953,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -996,13 +996,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1059,7 +1053,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1335,27 +1343,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA32"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7265625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.54296875" customWidth="1"/>
-    <col min="11" max="11" width="38.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="44.453125" style="12" customWidth="1"/>
-    <col min="13" max="14" width="38.7265625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" customWidth="1"/>
+    <col min="11" max="11" width="38.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="44.42578125" style="12" customWidth="1"/>
+    <col min="13" max="14" width="38.7109375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18" customHeight="1">
@@ -1415,7 +1423,7 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
     </row>
-    <row r="2" spans="1:27" ht="72.5">
+    <row r="2" spans="1:27" ht="75">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1472,7 +1480,7 @@
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
     </row>
-    <row r="3" spans="1:27" ht="87">
+    <row r="3" spans="1:27" ht="105">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1482,7 +1490,7 @@
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3">
@@ -1529,7 +1537,7 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" spans="1:27" ht="174">
+    <row r="4" spans="1:27" ht="195">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1586,7 +1594,7 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
     </row>
-    <row r="5" spans="1:27" ht="130.5">
+    <row r="5" spans="1:27" ht="135">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1643,7 +1651,7 @@
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
     </row>
-    <row r="6" spans="1:27" ht="188.5">
+    <row r="6" spans="1:27" ht="210">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1700,7 +1708,7 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
     </row>
-    <row r="7" spans="1:27" ht="116">
+    <row r="7" spans="1:27" ht="120">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1757,7 +1765,7 @@
       <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
     </row>
-    <row r="8" spans="1:27" ht="130.5">
+    <row r="8" spans="1:27" ht="135">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1814,7 +1822,7 @@
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
     </row>
-    <row r="9" spans="1:27" ht="87">
+    <row r="9" spans="1:27" ht="90">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1873,7 +1881,7 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
     </row>
-    <row r="10" spans="1:27" ht="116">
+    <row r="10" spans="1:27" ht="120">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1932,7 +1940,7 @@
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
     </row>
-    <row r="11" spans="1:27" ht="261">
+    <row r="11" spans="1:27" ht="285">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1989,7 +1997,7 @@
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
     </row>
-    <row r="12" spans="1:27" ht="130.5">
+    <row r="12" spans="1:27" ht="150">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2046,7 +2054,7 @@
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
     </row>
-    <row r="13" spans="1:27" ht="116">
+    <row r="13" spans="1:27" ht="120">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2103,7 +2111,7 @@
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
     </row>
-    <row r="14" spans="1:27" ht="87">
+    <row r="14" spans="1:27" ht="90">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2160,7 +2168,7 @@
       <c r="Z14" s="4"/>
       <c r="AA14" s="4"/>
     </row>
-    <row r="15" spans="1:27" ht="203">
+    <row r="15" spans="1:27" ht="210">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2217,7 +2225,7 @@
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
     </row>
-    <row r="16" spans="1:27" ht="116">
+    <row r="16" spans="1:27" ht="150">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2274,7 +2282,7 @@
       <c r="Z16" s="4"/>
       <c r="AA16" s="4"/>
     </row>
-    <row r="17" spans="1:27" ht="58">
+    <row r="17" spans="1:27" ht="60">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2331,7 +2339,7 @@
       <c r="Z17" s="4"/>
       <c r="AA17" s="4"/>
     </row>
-    <row r="18" spans="1:27" ht="116">
+    <row r="18" spans="1:27" ht="150">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2388,7 +2396,7 @@
       <c r="Z18" s="4"/>
       <c r="AA18" s="4"/>
     </row>
-    <row r="19" spans="1:27" ht="174">
+    <row r="19" spans="1:27" ht="210">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2445,7 +2453,7 @@
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
     </row>
-    <row r="20" spans="1:27" ht="130.5">
+    <row r="20" spans="1:27" ht="150">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2502,7 +2510,7 @@
       <c r="Z20" s="4"/>
       <c r="AA20" s="4"/>
     </row>
-    <row r="21" spans="1:27" ht="87">
+    <row r="21" spans="1:27" ht="90">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2559,7 +2567,7 @@
       <c r="Z21" s="4"/>
       <c r="AA21" s="4"/>
     </row>
-    <row r="22" spans="1:27" ht="101.5">
+    <row r="22" spans="1:27" ht="105">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2599,7 +2607,7 @@
       <c r="M22" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="N22" s="29"/>
+      <c r="N22" s="27"/>
       <c r="O22" s="4">
         <v>1</v>
       </c>
@@ -2616,7 +2624,7 @@
       <c r="Z22" s="4"/>
       <c r="AA22" s="4"/>
     </row>
-    <row r="23" spans="1:27" ht="232">
+    <row r="23" spans="1:27" ht="255">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2656,7 +2664,7 @@
       <c r="M23" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="N23" s="30"/>
+      <c r="N23" s="28"/>
       <c r="O23" s="4">
         <v>1</v>
       </c>
@@ -2673,7 +2681,7 @@
       <c r="Z23" s="4"/>
       <c r="AA23" s="4"/>
     </row>
-    <row r="24" spans="1:27" ht="87">
+    <row r="24" spans="1:27" ht="90">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2695,7 +2703,7 @@
       <c r="G24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="20" t="s">
         <v>22</v>
       </c>
       <c r="I24" s="2">
@@ -2704,21 +2712,21 @@
       <c r="J24" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K24" s="18" t="s">
+      <c r="K24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="L24" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="M24" s="19" t="s">
+      <c r="L24" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="M24" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="N24" s="31"/>
-      <c r="O24" s="34">
+      <c r="N24" s="29"/>
+      <c r="O24" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="174">
+    <row r="25" spans="1:27" ht="180">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2740,7 +2748,7 @@
       <c r="G25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="20" t="s">
         <v>22</v>
       </c>
       <c r="I25" s="2">
@@ -2749,7 +2757,7 @@
       <c r="J25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K25" s="20" t="s">
+      <c r="K25" s="18" t="s">
         <v>100</v>
       </c>
       <c r="L25" s="14" t="s">
@@ -2758,12 +2766,12 @@
       <c r="M25" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="N25" s="32"/>
-      <c r="O25" s="34">
+      <c r="N25" s="30"/>
+      <c r="O25" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="174">
+    <row r="26" spans="1:27" ht="195">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2776,7 +2784,7 @@
       <c r="D26" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="19">
         <v>2</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -2785,7 +2793,7 @@
       <c r="G26" s="2">
         <v>3</v>
       </c>
-      <c r="H26" s="22" t="s">
+      <c r="H26" s="20" t="s">
         <v>22</v>
       </c>
       <c r="I26" s="2">
@@ -2794,7 +2802,7 @@
       <c r="J26" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="K26" s="22" t="s">
+      <c r="K26" s="20" t="s">
         <v>108</v>
       </c>
       <c r="L26" s="14" t="s">
@@ -2803,12 +2811,12 @@
       <c r="M26" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="N26" s="32"/>
-      <c r="O26" s="34">
+      <c r="N26" s="30"/>
+      <c r="O26" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="174">
+    <row r="27" spans="1:27" ht="195">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2818,7 +2826,7 @@
       <c r="C27" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="20" t="s">
         <v>113</v>
       </c>
       <c r="E27" s="2">
@@ -2830,34 +2838,34 @@
       <c r="G27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="22" t="s">
+      <c r="H27" s="20" t="s">
         <v>22</v>
       </c>
       <c r="I27" s="2">
         <v>242</v>
       </c>
-      <c r="J27" s="27" t="s">
+      <c r="J27" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="K27" s="28" t="s">
+      <c r="K27" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="L27" s="23" t="s">
+      <c r="L27" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="M27" s="23" t="s">
+      <c r="M27" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="N27" s="33"/>
-      <c r="O27" s="34">
+      <c r="N27" s="31"/>
+      <c r="O27" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="101.5">
+    <row r="28" spans="1:27" ht="120">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="22" t="s">
         <v>116</v>
       </c>
       <c r="C28" s="14" t="s">
@@ -2875,7 +2883,7 @@
       <c r="G28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="20" t="s">
         <v>22</v>
       </c>
       <c r="I28" s="2">
@@ -2884,7 +2892,7 @@
       <c r="J28" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K28" s="35" t="s">
+      <c r="K28" s="33" t="s">
         <v>209</v>
       </c>
       <c r="L28" s="14" t="s">
@@ -2893,12 +2901,12 @@
       <c r="M28" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="N28" s="32"/>
-      <c r="O28" s="34">
+      <c r="N28" s="30"/>
+      <c r="O28" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="145">
+    <row r="29" spans="1:27" ht="165">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2929,7 +2937,7 @@
       <c r="J29" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="K29" s="22" t="s">
+      <c r="K29" s="20" t="s">
         <v>100</v>
       </c>
       <c r="L29" s="14" t="s">
@@ -2938,12 +2946,12 @@
       <c r="M29" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="N29" s="32"/>
-      <c r="O29" s="37">
+      <c r="N29" s="30"/>
+      <c r="O29" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="217.5">
+    <row r="30" spans="1:27" ht="225">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2974,21 +2982,21 @@
       <c r="J30" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="K30" s="22" t="s">
+      <c r="K30" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="L30" s="25" t="s">
+      <c r="L30" s="23" t="s">
         <v>132</v>
       </c>
       <c r="M30" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="N30" s="32"/>
-      <c r="O30" s="37">
+      <c r="N30" s="30"/>
+      <c r="O30" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="174">
+    <row r="31" spans="1:27" ht="180">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -3019,7 +3027,7 @@
       <c r="J31" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="K31" s="36" t="s">
+      <c r="K31" s="34" t="s">
         <v>210</v>
       </c>
       <c r="L31" s="14" t="s">
@@ -3028,26 +3036,311 @@
       <c r="M31" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="N31" s="32"/>
-      <c r="O31" s="37">
+      <c r="N31" s="30"/>
+      <c r="O31" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:27">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="15"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="38"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="38"/>
+      <c r="M36" s="38"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="38"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="38"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="38"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="38"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="38"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="38"/>
+      <c r="M42" s="38"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="38"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="38"/>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="38"/>
+      <c r="M45" s="38"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="39"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="38"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="39"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="38"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="39"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="39"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="39"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="38"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="39"/>
+      <c r="L51" s="38"/>
+      <c r="M51" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add AIPW and IPW, add all modification
only need to rerun tmle if asked
</commit_message>
<xml_diff>
--- a/cleaned_data/meta_data.xlsx
+++ b/cleaned_data/meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A29EE6-8E31-4083-A7F8-BCCC8B5FD865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E260BD-B6F0-4E7D-BC8A-F4E65BC90361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1299,9 +1299,6 @@
     <t>Block</t>
   </si>
   <si>
-    <t>Covariate Adaptive</t>
-  </si>
-  <si>
     <t>Stratified Block</t>
   </si>
   <si>
@@ -1342,9 +1339,6 @@
   </si>
   <si>
     <t>Critical Care</t>
-  </si>
-  <si>
-    <t>Cluster</t>
   </si>
   <si>
     <t>Hypertension</t>
@@ -1415,18 +1409,31 @@
   </si>
   <si>
     <t>Orthodontics</t>
+  </si>
+  <si>
+    <t>Biased Coin</t>
+  </si>
+  <si>
+    <t>Stratified Rerandomization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1675,156 +1682,171 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1832,63 +1854,49 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2169,10 +2177,10 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P33" sqref="P33"/>
+      <selection pane="bottomRight" activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2208,7 +2216,7 @@
         <v>29</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>30</v>
@@ -2241,7 +2249,7 @@
         <v>335</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>174</v>
@@ -2345,7 +2353,7 @@
         <v>337</v>
       </c>
       <c r="P3" s="65" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q3" s="9"/>
     </row>
@@ -2545,11 +2553,11 @@
       <c r="N7" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="O7" s="64" t="s">
-        <v>339</v>
+      <c r="O7" s="76" t="s">
+        <v>374</v>
       </c>
       <c r="P7" s="64" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Q7" s="9"/>
     </row>
@@ -2597,10 +2605,10 @@
         <v>312</v>
       </c>
       <c r="O8" s="67" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P8" s="65" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Q8" s="9"/>
     </row>
@@ -2651,7 +2659,7 @@
         <v>338</v>
       </c>
       <c r="P9" s="64" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q9" s="9" t="s">
         <v>175</v>
@@ -2701,7 +2709,7 @@
         <v>313</v>
       </c>
       <c r="O10" s="68" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P10" s="64" t="s">
         <v>315</v>
@@ -2754,7 +2762,7 @@
         <v>314</v>
       </c>
       <c r="O11" s="68" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P11" s="64" t="s">
         <v>318</v>
@@ -2802,13 +2810,13 @@
         <v>17</v>
       </c>
       <c r="N12" s="64" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="O12" s="64" t="s">
         <v>337</v>
       </c>
       <c r="P12" s="64" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q12" s="8"/>
     </row>
@@ -2857,7 +2865,7 @@
         <v>337</v>
       </c>
       <c r="P13" s="64" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="Q13" s="9"/>
     </row>
@@ -2956,10 +2964,10 @@
         <v>316</v>
       </c>
       <c r="O15" s="64" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P15" s="68" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="Q15" s="8"/>
     </row>
@@ -3010,7 +3018,7 @@
         <v>337</v>
       </c>
       <c r="P16" s="69" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="Q16" s="9"/>
     </row>
@@ -3061,7 +3069,7 @@
         <v>337</v>
       </c>
       <c r="P17" s="64" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Q17" s="8"/>
     </row>
@@ -3112,7 +3120,7 @@
         <v>337</v>
       </c>
       <c r="P18" s="64" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Q18" s="8"/>
     </row>
@@ -3211,10 +3219,10 @@
         <v>310</v>
       </c>
       <c r="O20" s="64" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P20" s="49" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q20" s="8"/>
     </row>
@@ -3265,7 +3273,7 @@
         <v>338</v>
       </c>
       <c r="P21" s="64" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q21" s="8"/>
     </row>
@@ -3365,7 +3373,7 @@
         <v>337</v>
       </c>
       <c r="P23" s="64" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q23" s="25"/>
     </row>
@@ -3416,7 +3424,7 @@
         <v>337</v>
       </c>
       <c r="P24" s="64" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="Q24" s="14"/>
     </row>
@@ -3667,11 +3675,11 @@
       <c r="N29" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="O29" s="64" t="s">
-        <v>354</v>
+      <c r="O29" s="76" t="s">
+        <v>375</v>
       </c>
       <c r="P29" s="64" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="Q29" s="12"/>
     </row>
@@ -3719,7 +3727,7 @@
         <v>321</v>
       </c>
       <c r="O30" s="68" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P30" s="59" t="s">
         <v>317</v>
@@ -3773,7 +3781,7 @@
         <v>337</v>
       </c>
       <c r="P31" s="64" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Q31" s="12"/>
     </row>
@@ -3822,7 +3830,7 @@
         <v>337</v>
       </c>
       <c r="P32" s="72" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Q32" s="25"/>
     </row>
@@ -3831,13 +3839,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="73" t="s">
+        <v>366</v>
+      </c>
+      <c r="C33" s="74" t="s">
+        <v>367</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>368</v>
-      </c>
-      <c r="C33" s="74" t="s">
-        <v>369</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>370</v>
       </c>
       <c r="E33" s="1">
         <v>2021</v>
@@ -3846,7 +3854,7 @@
         <v>3</v>
       </c>
       <c r="G33" s="73" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H33" s="75" t="s">
         <v>35</v>
@@ -3855,16 +3863,16 @@
         <v>57</v>
       </c>
       <c r="J33" s="73" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K33" s="73" t="s">
         <v>37</v>
       </c>
       <c r="L33" s="74" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="M33" s="74" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N33" s="72" t="s">
         <v>309</v>
@@ -3873,7 +3881,7 @@
         <v>337</v>
       </c>
       <c r="P33" s="72" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="Q33" s="25"/>
     </row>
@@ -3922,7 +3930,7 @@
         <v>336</v>
       </c>
       <c r="P34" s="64" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="Q34" s="25"/>
     </row>
@@ -3973,7 +3981,7 @@
         <v>338</v>
       </c>
       <c r="P35" s="68" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q35" s="25"/>
     </row>
@@ -4024,7 +4032,7 @@
         <v>338</v>
       </c>
       <c r="P36" s="64" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q36" s="25"/>
     </row>
@@ -4072,7 +4080,7 @@
         <v>323</v>
       </c>
       <c r="O37" s="68" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P37" s="64" t="s">
         <v>319</v>
@@ -4126,7 +4134,7 @@
         <v>336</v>
       </c>
       <c r="P38" s="64" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="Q38" s="25"/>
     </row>
@@ -4171,10 +4179,10 @@
         <v>215</v>
       </c>
       <c r="N39" s="64" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="O39" s="64" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P39" s="64" t="s">
         <v>317</v>
@@ -4225,10 +4233,10 @@
         <v>325</v>
       </c>
       <c r="O40" s="68" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P40" s="64" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Q40" s="25"/>
     </row>
@@ -4426,13 +4434,13 @@
         <v>245</v>
       </c>
       <c r="N44" s="64" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="O44" s="64" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P44" s="68" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q44" s="25"/>
     </row>
@@ -4534,7 +4542,7 @@
         <v>336</v>
       </c>
       <c r="P46" s="64" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="Q46" s="25"/>
     </row>
@@ -4683,7 +4691,7 @@
         <v>338</v>
       </c>
       <c r="P49" s="68" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="Q49" s="25"/>
     </row>
@@ -4731,7 +4739,7 @@
         <v>331</v>
       </c>
       <c r="O50" s="68" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P50" s="60" t="s">
         <v>330</v>
@@ -4779,13 +4787,13 @@
         <v>301</v>
       </c>
       <c r="N51" s="68" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="O51" s="68" t="s">
         <v>336</v>
       </c>
       <c r="P51" s="64" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="Q51" s="25"/>
     </row>

</xml_diff>